<commit_message>
Bitmasks complete for all required operations
</commit_message>
<xml_diff>
--- a/OP to Binary.xlsx
+++ b/OP to Binary.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\La Nerderia\Documents\UWB\Fall 2014\CSS 422\Disassembler\fractions-of-a-penny\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="107">
   <si>
     <t>Assembly Operation</t>
   </si>
@@ -241,13 +246,112 @@
   </si>
   <si>
     <t>d-Displacemnt</t>
+  </si>
+  <si>
+    <t>B000</t>
+  </si>
+  <si>
+    <t>81C0</t>
+  </si>
+  <si>
+    <t>41C0</t>
+  </si>
+  <si>
+    <t>C1C0</t>
+  </si>
+  <si>
+    <t>01C0</t>
+  </si>
+  <si>
+    <t>0C00</t>
+  </si>
+  <si>
+    <t>6D00</t>
+  </si>
+  <si>
+    <t>6C00</t>
+  </si>
+  <si>
+    <t>6500</t>
+  </si>
+  <si>
+    <t>6800</t>
+  </si>
+  <si>
+    <t>E000</t>
+  </si>
+  <si>
+    <t>E100</t>
+  </si>
+  <si>
+    <t>E008</t>
+  </si>
+  <si>
+    <t>E108</t>
+  </si>
+  <si>
+    <t>E018</t>
+  </si>
+  <si>
+    <t>E118</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>3040</t>
+  </si>
+  <si>
+    <t>2040</t>
+  </si>
+  <si>
+    <t>4880</t>
+  </si>
+  <si>
+    <t>4E71</t>
+  </si>
+  <si>
+    <t>4E75</t>
+  </si>
+  <si>
+    <t>4E80</t>
+  </si>
+  <si>
+    <t>4400</t>
+  </si>
+  <si>
+    <t>D000</t>
+  </si>
+  <si>
+    <t>D0C0</t>
+  </si>
+  <si>
+    <t>Bitmasks</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -287,13 +391,25 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -388,7 +504,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -396,6 +512,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -482,9 +608,181 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:F42" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A9:F42"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Operation" dataDxfId="7"/>
+    <tableColumn id="2" name="Binary" dataDxfId="6"/>
+    <tableColumn id="3" name="Column1" dataDxfId="5"/>
+    <tableColumn id="4" name="Column2" dataDxfId="4"/>
+    <tableColumn id="5" name="Column3" dataDxfId="3"/>
+    <tableColumn id="6" name="Bitmasks" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -809,61 +1107,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
-    <col min="2" max="5" width="6.83203125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="10.25" style="2" customWidth="1"/>
+    <col min="3" max="5" width="11.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="3" customWidth="1"/>
+    <col min="7" max="12" width="10.875" style="3"/>
+    <col min="13" max="13" width="11.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -878,9 +1200,16 @@
       <c r="E10" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -895,9 +1224,16 @@
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
+      <c r="F11" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -912,9 +1248,16 @@
       <c r="E12" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
+      <c r="F12" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -929,9 +1272,16 @@
       <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
+      <c r="F13" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -946,9 +1296,16 @@
       <c r="E14" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="3" t="s">
+      <c r="F14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -957,14 +1314,21 @@
       <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>52</v>
+      <c r="D15" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -980,8 +1344,15 @@
       <c r="E16" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
@@ -997,8 +1368,15 @@
       <c r="E17" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1014,8 +1392,15 @@
       <c r="E18" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="6"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
@@ -1031,8 +1416,15 @@
       <c r="E19" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="6"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -1048,8 +1440,15 @@
       <c r="E20" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="9">
+        <v>8000</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -1065,8 +1464,15 @@
       <c r="E21" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="9">
+        <v>9000</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -1082,8 +1488,15 @@
       <c r="E22" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="6"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1099,8 +1512,15 @@
       <c r="E23" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1116,8 +1536,15 @@
       <c r="E24" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -1133,8 +1560,15 @@
       <c r="E25" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="9">
+        <v>5100</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="N25" s="9"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1150,8 +1584,15 @@
       <c r="E26" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="9">
+        <v>6000</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="N26" s="9"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -1167,8 +1608,15 @@
       <c r="E27" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -1184,8 +1632,15 @@
       <c r="E28" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="N28" s="8"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1201,8 +1656,15 @@
       <c r="E29" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="N29" s="8"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
@@ -1218,8 +1680,15 @@
       <c r="E30" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="N30" s="8"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
@@ -1235,8 +1704,15 @@
       <c r="E31" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
@@ -1252,8 +1728,15 @@
       <c r="E32" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="N32" s="8"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
@@ -1269,8 +1752,15 @@
       <c r="E33" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="2"/>
+      <c r="N33" s="8"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -1286,8 +1776,15 @@
       <c r="E34" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="2"/>
+      <c r="N34" s="8"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
@@ -1303,8 +1800,15 @@
       <c r="E35" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="2"/>
+      <c r="N35" s="8"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
@@ -1320,8 +1824,15 @@
       <c r="E36" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="2"/>
+      <c r="N36" s="8"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>40</v>
       </c>
@@ -1337,8 +1848,15 @@
       <c r="E37" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="N37" s="8"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>41</v>
       </c>
@@ -1354,8 +1872,15 @@
       <c r="E38" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="N38" s="8"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>42</v>
       </c>
@@ -1371,8 +1896,15 @@
       <c r="E39" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="N39" s="8"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
@@ -1388,8 +1920,15 @@
       <c r="E40" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="N40" s="8"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>46</v>
       </c>
@@ -1405,8 +1944,15 @@
       <c r="E41" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="N41" s="8"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
@@ -1422,10 +1968,23 @@
       <c r="E42" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="F42" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="6"/>
+      <c r="N42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F13 F10:F12 F24 F28:F29 F37:F42" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Excel file updated with EA1 opcodes for shifts and rotates.  Excel file updated as well, with highlighting to show added bitmasks
</commit_message>
<xml_diff>
--- a/OP to Binary.xlsx
+++ b/OP to Binary.xlsx
@@ -14,17 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="112">
   <si>
     <t>Assembly Operation</t>
   </si>
@@ -119,27 +114,9 @@
     <t>BGE</t>
   </si>
   <si>
-    <t>ASR</t>
-  </si>
-  <si>
     <t>1110</t>
   </si>
   <si>
-    <t>ASL</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>LSL</t>
-  </si>
-  <si>
-    <t>ROR</t>
-  </si>
-  <si>
-    <t>ROL</t>
-  </si>
-  <si>
     <t>MOVEM</t>
   </si>
   <si>
@@ -324,6 +301,60 @@
   </si>
   <si>
     <t>Decimal</t>
+  </si>
+  <si>
+    <t>ROL E6</t>
+  </si>
+  <si>
+    <t>ROL E1</t>
+  </si>
+  <si>
+    <t>E6C0</t>
+  </si>
+  <si>
+    <t>E7C0</t>
+  </si>
+  <si>
+    <t>ROR E6</t>
+  </si>
+  <si>
+    <t>ROR E1</t>
+  </si>
+  <si>
+    <t>LSL E6</t>
+  </si>
+  <si>
+    <t>LSL E1</t>
+  </si>
+  <si>
+    <t>LSR E1</t>
+  </si>
+  <si>
+    <t>LSR E6</t>
+  </si>
+  <si>
+    <t>E3C0</t>
+  </si>
+  <si>
+    <t>E2C0</t>
+  </si>
+  <si>
+    <t>ASL E6</t>
+  </si>
+  <si>
+    <t>ASR E6</t>
+  </si>
+  <si>
+    <t>ASL E1</t>
+  </si>
+  <si>
+    <t>E1C0</t>
+  </si>
+  <si>
+    <t>ASR E1</t>
+  </si>
+  <si>
+    <t>E0C0</t>
   </si>
 </sst>
 </file>
@@ -377,15 +408,21 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -393,6 +430,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -477,7 +523,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -493,6 +539,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -578,43 +637,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -743,6 +765,43 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
@@ -757,19 +816,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:G42" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A9:G42"/>
-  <sortState ref="A10:G42">
-    <sortCondition descending="1" ref="G9:G42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:G48" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A9:G48"/>
+  <sortState ref="A10:G48">
+    <sortCondition descending="1" ref="G9:G48"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="OPCode" dataDxfId="8"/>
-    <tableColumn id="2" name="2^3" dataDxfId="7"/>
-    <tableColumn id="3" name="2^2" dataDxfId="6"/>
-    <tableColumn id="4" name="2^1" dataDxfId="5"/>
-    <tableColumn id="5" name="2^0" dataDxfId="4"/>
-    <tableColumn id="6" name="Hex" dataDxfId="3"/>
-    <tableColumn id="7" name="Decimal" dataDxfId="2">
+    <tableColumn id="1" name="OPCode" dataDxfId="6"/>
+    <tableColumn id="2" name="2^3" dataDxfId="5"/>
+    <tableColumn id="3" name="2^2" dataDxfId="4"/>
+    <tableColumn id="4" name="2^1" dataDxfId="3"/>
+    <tableColumn id="5" name="2^0" dataDxfId="2"/>
+    <tableColumn id="6" name="Hex" dataDxfId="1"/>
+    <tableColumn id="7" name="Decimal" dataDxfId="0">
       <calculatedColumnFormula>HEX2DEC(F10)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1099,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1111,861 +1170,1051 @@
     <col min="2" max="5" width="6.875" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="3"/>
+    <col min="8" max="8" width="10.875" style="3"/>
+    <col min="9" max="9" width="11.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1100</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="11">
+        <f>HEX2DEC(F10)</f>
+        <v>59328</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1110</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1100</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="14">
+        <f>HEX2DEC(F11)</f>
+        <v>59072</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="14">
+        <f>HEX2DEC(F12)</f>
+        <v>58304</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="14">
+        <f>HEX2DEC(F13)</f>
+        <v>58048</v>
+      </c>
+      <c r="I13" s="3" t="str">
+        <f>BIN2HEX(I12)</f>
+        <v>E</v>
+      </c>
+      <c r="J13" s="3" t="str">
+        <f>BIN2HEX(J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="3" t="str">
+        <f>BIN2HEX(K12)</f>
+        <v>C</v>
+      </c>
+      <c r="L13" s="3" t="str">
+        <f>BIN2HEX(L12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="14">
+        <f>HEX2DEC(F14)</f>
+        <v>57792</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="3">
-        <f>HEX2DEC(F10)</f>
-        <v>57624</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="3">
-        <f>HEX2DEC(F11)</f>
-        <v>57608</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="3">
-        <f>HEX2DEC(F12)</f>
-        <v>57600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="3">
-        <f>HEX2DEC(F13)</f>
-        <v>57368</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="3">
-        <f>HEX2DEC(F14)</f>
-        <v>57352</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G15" s="3">
         <f>HEX2DEC(F15)</f>
-        <v>57344</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57624</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G16" s="3">
         <f>HEX2DEC(F16)</f>
-        <v>53440</v>
+        <v>57608</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F17" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G17" s="3">
         <f>HEX2DEC(F17)</f>
-        <v>53248</v>
+        <v>57600</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="E18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="14">
         <f>HEX2DEC(F18)</f>
-        <v>49600</v>
+        <v>57536</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G19" s="3">
         <f>HEX2DEC(F19)</f>
-        <v>45056</v>
+        <v>57368</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>103</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="7">
-        <v>9000</v>
+        <v>54</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="G20" s="3">
         <f>HEX2DEC(F20)</f>
-        <v>36864</v>
+        <v>57352</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G21" s="3">
         <f>HEX2DEC(F21)</f>
-        <v>33216</v>
+        <v>57344</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="7">
-        <v>8000</v>
+        <v>43</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="G22" s="3">
         <f>HEX2DEC(F22)</f>
-        <v>32768</v>
+        <v>53440</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="G23" s="3">
         <f>HEX2DEC(F23)</f>
-        <v>27904</v>
+        <v>53248</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G24" s="3">
         <f>HEX2DEC(F24)</f>
-        <v>27648</v>
+        <v>49600</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="7">
-        <v>6800</v>
+        <v>43</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="G25" s="3">
         <f>HEX2DEC(F25)</f>
-        <v>26624</v>
+        <v>45056</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F26" s="7">
-        <v>6500</v>
+        <v>9000</v>
       </c>
       <c r="G26" s="3">
         <f>HEX2DEC(F26)</f>
-        <v>25856</v>
+        <v>36864</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="7">
-        <v>6000</v>
+        <v>43</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="G27" s="3">
         <f>HEX2DEC(F27)</f>
-        <v>24576</v>
+        <v>33216</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F28" s="7">
-        <v>5100</v>
+        <v>8000</v>
       </c>
       <c r="G28" s="3">
         <f>HEX2DEC(F28)</f>
-        <v>20736</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G29" s="3">
         <f>HEX2DEC(F29)</f>
-        <v>20096</v>
+        <v>27904</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>2</v>
+        <v>30</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="G30" s="3">
         <f>HEX2DEC(F30)</f>
-        <v>20085</v>
+        <v>27648</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>89</v>
+        <v>49</v>
+      </c>
+      <c r="F31" s="7">
+        <v>6800</v>
       </c>
       <c r="G31" s="3">
         <f>HEX2DEC(F31)</f>
-        <v>20081</v>
+        <v>26624</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F32" s="7">
-        <v>4880</v>
+        <v>6500</v>
       </c>
       <c r="G32" s="3">
         <f>HEX2DEC(F32)</f>
-        <v>18560</v>
+        <v>25856</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F33" s="7">
-        <v>4400</v>
+        <v>6000</v>
       </c>
       <c r="G33" s="3">
         <f>HEX2DEC(F33)</f>
-        <v>17408</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>78</v>
+        <v>43</v>
+      </c>
+      <c r="F34" s="7">
+        <v>5100</v>
       </c>
       <c r="G34" s="3">
         <f>HEX2DEC(F34)</f>
-        <v>16832</v>
+        <v>20736</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="7">
-        <v>3040</v>
+      <c r="F35" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="G35" s="3">
         <f>HEX2DEC(F35)</f>
-        <v>12352</v>
+        <v>20096</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="7">
-        <v>3000</v>
+        <v>24</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="G36" s="3">
         <f>HEX2DEC(F36)</f>
-        <v>12288</v>
+        <v>20085</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" s="7">
-        <v>2040</v>
+        <v>33</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="G37" s="3">
         <f>HEX2DEC(F37)</f>
-        <v>8256</v>
+        <v>20081</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F38" s="7">
-        <v>2000</v>
+        <v>4880</v>
       </c>
       <c r="G38" s="3">
         <f>HEX2DEC(F38)</f>
-        <v>8192</v>
+        <v>18560</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F39" s="7">
-        <v>1000</v>
+        <v>4400</v>
       </c>
       <c r="G39" s="3">
         <f>HEX2DEC(F39)</f>
-        <v>4096</v>
+        <v>17408</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G40" s="3">
         <f>HEX2DEC(F40)</f>
-        <v>3072</v>
+        <v>16832</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>80</v>
+        <v>43</v>
+      </c>
+      <c r="F41" s="7">
+        <v>3040</v>
       </c>
       <c r="G41" s="3">
         <f>HEX2DEC(F41)</f>
-        <v>448</v>
+        <v>12352</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="F42" s="7">
+        <v>3000</v>
       </c>
       <c r="G42" s="3">
         <f>HEX2DEC(F42)</f>
+        <v>12288</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" s="7">
+        <v>2040</v>
+      </c>
+      <c r="G43" s="3">
+        <f>HEX2DEC(F43)</f>
+        <v>8256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G44" s="3">
+        <f>HEX2DEC(F44)</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G45" s="3">
+        <f>HEX2DEC(F45)</f>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G46" s="3">
+        <f>HEX2DEC(F46)</f>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="3">
+        <f>HEX2DEC(F47)</f>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" s="3">
+        <f>HEX2DEC(F48)</f>
         <v>0</v>
       </c>
     </row>
@@ -1975,10 +2224,5 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>